<commit_message>
Added prep for Kalman smoothing model & additionally added expected inflations data and forecasting (v0.09)
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C173D2-BA63-49D8-B89F-B11D80D573E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E78C1B-767B-4647-AC1A-7F991C173F91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
-    <sheet name="history_params" sheetId="2" r:id="rId1"/>
+    <sheet name="params" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="135">
   <si>
     <t>gdp</t>
   </si>
@@ -124,9 +124,6 @@
     <t>GDPC1</t>
   </si>
   <si>
-    <t>stationary</t>
-  </si>
-  <si>
     <t>dlog</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>freq</t>
   </si>
   <si>
-    <t>fred</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -184,9 +178,6 @@
     <t>CSUSHPISA</t>
   </si>
   <si>
-    <t>nc</t>
-  </si>
-  <si>
     <t>dfm</t>
   </si>
   <si>
@@ -271,21 +262,200 @@
     <t>advsales</t>
   </si>
   <si>
-    <t>RSFXMV</t>
-  </si>
-  <si>
     <t>kclfi</t>
   </si>
   <si>
     <t>FRBKCLMCILA</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>VIX</t>
+  </si>
+  <si>
+    <t>Case-Shiller Housing Price Index</t>
+  </si>
+  <si>
+    <t>Effective Federal Funds Rate</t>
+  </si>
+  <si>
+    <t>Secured Overnight Financing Rate</t>
+  </si>
+  <si>
+    <t>Treasury Yield 10Y</t>
+  </si>
+  <si>
+    <t>Treasury Yield 30Y</t>
+  </si>
+  <si>
+    <t>Treasury Yield 20Y</t>
+  </si>
+  <si>
+    <t>Treasury Yield 5Y</t>
+  </si>
+  <si>
+    <t>Treasury Yield 2Y</t>
+  </si>
+  <si>
+    <t>Treasury Yield 7Y</t>
+  </si>
+  <si>
+    <t>Treasury Yield 1Y</t>
+  </si>
+  <si>
+    <t>Treasury Yield 6M</t>
+  </si>
+  <si>
+    <t>Treasury Yield 3M</t>
+  </si>
+  <si>
+    <t>Treasury Yield 1M</t>
+  </si>
+  <si>
+    <t>Vehicle Sales</t>
+  </si>
+  <si>
+    <t>Unemployment rate</t>
+  </si>
+  <si>
+    <t>Weekly Economic Index</t>
+  </si>
+  <si>
+    <t>S&amp;P 500</t>
+  </si>
+  <si>
+    <t>Outstanding Real Estate Loans</t>
+  </si>
+  <si>
+    <t>Outstanding Credit Card Balances</t>
+  </si>
+  <si>
+    <t>Housing Prices: New Listed Prices</t>
+  </si>
+  <si>
+    <t>St. Louis Fed Financial Stress Index</t>
+  </si>
+  <si>
+    <t>U.S. Dollar Index</t>
+  </si>
+  <si>
+    <t>ncmethod</t>
+  </si>
+  <si>
+    <t>csent</t>
+  </si>
+  <si>
+    <t>Consumer Confidence (OECD)</t>
+  </si>
+  <si>
+    <t>CSCICP03USM665S</t>
+  </si>
+  <si>
+    <t>indpro</t>
+  </si>
+  <si>
+    <t>Industrial Production index</t>
+  </si>
+  <si>
+    <t>INDPRO</t>
+  </si>
+  <si>
+    <t>pce</t>
+  </si>
+  <si>
+    <t>PCE</t>
+  </si>
+  <si>
+    <t>dpi</t>
+  </si>
+  <si>
+    <t>DSPIC96</t>
+  </si>
+  <si>
+    <t>Real Disposable Personal Income</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Average Weeks Unemployed</t>
+  </si>
+  <si>
+    <t>RRSFS</t>
+  </si>
+  <si>
+    <t>Retail &amp; Food Sales</t>
+  </si>
+  <si>
+    <t>KC Fed Labor Market Index</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>millions of 1982-84 dollars</t>
+  </si>
+  <si>
+    <t>billions of 2012 dollars</t>
+  </si>
+  <si>
+    <t>pcepi</t>
+  </si>
+  <si>
+    <t>PCEPI</t>
+  </si>
+  <si>
+    <t>PCE Price Index</t>
+  </si>
+  <si>
+    <t>index 2012=100</t>
+  </si>
+  <si>
+    <t>dfminputs</t>
+  </si>
+  <si>
+    <t>dfmkey</t>
+  </si>
+  <si>
+    <t>fredname</t>
+  </si>
+  <si>
+    <t>stat_transform</t>
+  </si>
+  <si>
+    <t>key_input</t>
+  </si>
+  <si>
+    <t>PCEC96</t>
+  </si>
+  <si>
+    <t>apchg</t>
+  </si>
+  <si>
+    <t>display_transform</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -313,15 +483,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -332,6 +528,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B617FE1-E1E8-47F6-ABDE-CBCD504EF9D5}" name="Table1" displayName="Table1" ref="A1:M33" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:M33" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{60AC762C-6D0B-4264-8E22-97F42B37CA94}" name="varname"/>
+    <tableColumn id="9" xr3:uid="{3D1FA503-3E60-4701-ABF7-5AF7BEE6DD85}" name="fullname"/>
+    <tableColumn id="2" xr3:uid="{47D8E6E2-3F96-4CD3-A6C7-006EBA2077F7}" name="fredname"/>
+    <tableColumn id="12" xr3:uid="{78E77ED3-181C-477E-B64E-221C0A3DA799}" name="units"/>
+    <tableColumn id="3" xr3:uid="{E060E0B9-F2B0-4B1B-96FF-C5F9CEDB6EAC}" name="freq"/>
+    <tableColumn id="4" xr3:uid="{1C35A57C-07E1-44AF-A3A8-BA4148FF470E}" name="stat_transform"/>
+    <tableColumn id="13" xr3:uid="{A2B6536A-3838-480C-B021-497CABEA8F6B}" name="display_transform"/>
+    <tableColumn id="5" xr3:uid="{09B41ECC-5C41-4138-AE69-78C9F04DA2CB}" name="key_input"/>
+    <tableColumn id="6" xr3:uid="{70F5F520-6627-41D5-AAD0-C205290865FA}" name="nctype"/>
+    <tableColumn id="7" xr3:uid="{540373FC-A4BB-468A-8BAA-4A93D0B1A122}" name="sa"/>
+    <tableColumn id="8" xr3:uid="{C429D8D4-AEFE-4CFC-B8DA-223FB223EEB7}" name="dfminputs"/>
+    <tableColumn id="10" xr3:uid="{73F42D88-EBC6-4C98-862C-8700FC2B4625}" name="dfmkey"/>
+    <tableColumn id="11" xr3:uid="{6D9259C5-C493-44AF-8751-315AF6A8ACEB}" name="ncmethod"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -631,478 +849,848 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C7B812-9642-4C06-A80C-86E8497E4ACA}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
       <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>122</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>133</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>54</v>
       </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
         <v>55</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s">
         <v>57</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
         <v>61</v>
       </c>
-      <c r="B20" t="s">
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>133</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>62</v>
       </c>
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
         <v>63</v>
       </c>
-      <c r="B21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" t="s">
+        <v>133</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>66</v>
       </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>133</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>72</v>
       </c>
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>74</v>
       </c>
-      <c r="C25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" t="s">
+        <v>133</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>75</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" t="b">
-        <v>1</v>
+      <c r="D30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" t="s">
+        <v>133</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added GDP subcomponents import (v0.10)
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E78C1B-767B-4647-AC1A-7F991C173F91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0869014-1EE5-4B44-A9FE-74C9BD097396}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="3240" yWindow="1440" windowWidth="21600" windowHeight="11385" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="207">
   <si>
     <t>gdp</t>
   </si>
@@ -440,6 +441,222 @@
   </si>
   <si>
     <t>display_transform</t>
+  </si>
+  <si>
+    <t>GPDIC1</t>
+  </si>
+  <si>
+    <t>pdi</t>
+  </si>
+  <si>
+    <t>Food and beverages purchased for off-premises consumption</t>
+  </si>
+  <si>
+    <t>Exports</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>Government consumption expenditures and gross investment</t>
+  </si>
+  <si>
+    <t>Federal</t>
+  </si>
+  <si>
+    <t>State and local</t>
+  </si>
+  <si>
+    <t>PCECC96</t>
+  </si>
+  <si>
+    <t>DGDSRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>PCDGCC96</t>
+  </si>
+  <si>
+    <t>PCNDGC96</t>
+  </si>
+  <si>
+    <t>DFXARX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>PCESVC96</t>
+  </si>
+  <si>
+    <t>DHUTRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DHLCRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DTRSRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DRCARX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DFSARX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DIFSRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DOTSRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DNPIRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>PNFIC1</t>
+  </si>
+  <si>
+    <t>PRFIC1</t>
+  </si>
+  <si>
+    <t>CBIC1</t>
+  </si>
+  <si>
+    <t>NETEXC</t>
+  </si>
+  <si>
+    <t>B020RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>B021RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>GCEC1</t>
+  </si>
+  <si>
+    <t>FGCEC1</t>
+  </si>
+  <si>
+    <t>SLCEC1</t>
+  </si>
+  <si>
+    <t>pceq</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures</t>
+  </si>
+  <si>
+    <t>pceg</t>
+  </si>
+  <si>
+    <t>pcegn</t>
+  </si>
+  <si>
+    <t>pcegd</t>
+  </si>
+  <si>
+    <t>pcegf</t>
+  </si>
+  <si>
+    <t>pces</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Goods</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Nondurable Goods</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Durable Goods</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services</t>
+  </si>
+  <si>
+    <t>pceshousing</t>
+  </si>
+  <si>
+    <t>pcestransportation</t>
+  </si>
+  <si>
+    <t>pcesfood</t>
+  </si>
+  <si>
+    <t>pcesother</t>
+  </si>
+  <si>
+    <t>pcesfinal</t>
+  </si>
+  <si>
+    <t>pceshealth</t>
+  </si>
+  <si>
+    <t>pceschange</t>
+  </si>
+  <si>
+    <t>pcesrec</t>
+  </si>
+  <si>
+    <t>pcesnonprofit</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services: Housing &amp; Utilities</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services: Health Care</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services: Transportation</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services: Recreation</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services: Food Services &amp; Accomodations</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services: Financial Services</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services: Other Services</t>
+  </si>
+  <si>
+    <t>Personal Consumption Expenditures: Services: Nonprofit Services</t>
+  </si>
+  <si>
+    <t>Gross Private Domestic Investment</t>
+  </si>
+  <si>
+    <t>pdinr</t>
+  </si>
+  <si>
+    <t>pdir</t>
+  </si>
+  <si>
+    <t>Gross Private Domestic Investment: Nonresidential Investment</t>
+  </si>
+  <si>
+    <t>Gross Private Domestic Investment: Residential Investment</t>
+  </si>
+  <si>
+    <t>Gross Private Domestic Investment: Change in Private Inventories</t>
+  </si>
+  <si>
+    <t>nx</t>
+  </si>
+  <si>
+    <t>Net Exports</t>
+  </si>
+  <si>
+    <t>ex</t>
+  </si>
+  <si>
+    <t>im</t>
+  </si>
+  <si>
+    <t>govt</t>
+  </si>
+  <si>
+    <t>govtf</t>
+  </si>
+  <si>
+    <t>govts</t>
   </si>
 </sst>
 </file>
@@ -531,8 +748,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B617FE1-E1E8-47F6-ABDE-CBCD504EF9D5}" name="Table1" displayName="Table1" ref="A1:M33" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:M33" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B617FE1-E1E8-47F6-ABDE-CBCD504EF9D5}" name="Table1" displayName="Table1" ref="A1:M57" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:M57" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{60AC762C-6D0B-4264-8E22-97F42B37CA94}" name="varname"/>
     <tableColumn id="9" xr3:uid="{3D1FA503-3E60-4701-ABF7-5AF7BEE6DD85}" name="fullname"/>
@@ -849,15 +1066,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C7B812-9642-4C06-A80C-86E8497E4ACA}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
   </cols>
@@ -934,19 +1153,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
         <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -957,674 +1176,655 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="D4" t="s">
         <v>122</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L8" t="b">
-        <v>1</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>182</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>152</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>179</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="D13" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="D16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>205</v>
+      </c>
+      <c r="B25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" t="s">
+        <v>47</v>
+      </c>
+      <c r="M29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
         <v>115</v>
       </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" t="s">
-        <v>30</v>
-      </c>
-      <c r="K18" t="b">
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" t="b">
-        <v>1</v>
-      </c>
-      <c r="L19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" t="s">
-        <v>30</v>
-      </c>
-      <c r="K22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" t="s">
-        <v>133</v>
-      </c>
-      <c r="K23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" t="s">
-        <v>133</v>
-      </c>
-      <c r="K24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" t="s">
-        <v>133</v>
-      </c>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" t="s">
-        <v>30</v>
-      </c>
-      <c r="K26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" t="s">
-        <v>30</v>
-      </c>
-      <c r="K27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28" t="s">
-        <v>30</v>
-      </c>
-      <c r="K28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G29" t="s">
-        <v>133</v>
-      </c>
-      <c r="K29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C30" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
-      </c>
-      <c r="E30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" t="s">
-        <v>30</v>
       </c>
       <c r="K30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>115</v>
       </c>
       <c r="E31" t="s">
         <v>44</v>
@@ -1635,53 +1835,624 @@
       <c r="G31" t="s">
         <v>30</v>
       </c>
-      <c r="K31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>115</v>
       </c>
       <c r="E32" t="s">
         <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G32" t="s">
-        <v>133</v>
+        <v>30</v>
       </c>
       <c r="K32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
+      <c r="L43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>30</v>
+      </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" t="s">
+        <v>30</v>
+      </c>
+      <c r="K46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" t="s">
+        <v>133</v>
+      </c>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" t="s">
+        <v>133</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" t="s">
+        <v>133</v>
+      </c>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" t="s">
+        <v>30</v>
+      </c>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" t="s">
+        <v>30</v>
+      </c>
+      <c r="K51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" t="s">
+        <v>30</v>
+      </c>
+      <c r="K52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" t="s">
+        <v>121</v>
+      </c>
+      <c r="E53" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" t="s">
+        <v>29</v>
+      </c>
+      <c r="G53" t="s">
+        <v>133</v>
+      </c>
+      <c r="K53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" t="s">
+        <v>30</v>
+      </c>
+      <c r="K54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" t="s">
+        <v>30</v>
+      </c>
+      <c r="K55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="E56" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" t="s">
+        <v>133</v>
+      </c>
+      <c r="K56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>123</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B57" t="s">
         <v>125</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C57" t="s">
         <v>124</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D57" t="s">
         <v>126</v>
       </c>
-      <c r="E33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="E57" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1771,5 +2542,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C702AB-733A-4F06-A26B-F3AA9CF0214F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added dynamic fractor models & filtration code (v0.10)
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0869014-1EE5-4B44-A9FE-74C9BD097396}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56644670-DA89-4A7F-88DB-B6DE7A984CF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="1440" windowWidth="21600" windowHeight="11385" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="29730" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
@@ -419,9 +419,6 @@
     <t>index 2012=100</t>
   </si>
   <si>
-    <t>dfminputs</t>
-  </si>
-  <si>
     <t>dfmkey</t>
   </si>
   <si>
@@ -657,6 +654,9 @@
   </si>
   <si>
     <t>govts</t>
+  </si>
+  <si>
+    <t>dfminput</t>
   </si>
 </sst>
 </file>
@@ -761,7 +761,7 @@
     <tableColumn id="5" xr3:uid="{09B41ECC-5C41-4138-AE69-78C9F04DA2CB}" name="key_input"/>
     <tableColumn id="6" xr3:uid="{70F5F520-6627-41D5-AAD0-C205290865FA}" name="nctype"/>
     <tableColumn id="7" xr3:uid="{540373FC-A4BB-468A-8BAA-4A93D0B1A122}" name="sa"/>
-    <tableColumn id="8" xr3:uid="{C429D8D4-AEFE-4CFC-B8DA-223FB223EEB7}" name="dfminputs"/>
+    <tableColumn id="8" xr3:uid="{C429D8D4-AEFE-4CFC-B8DA-223FB223EEB7}" name="dfminput"/>
     <tableColumn id="10" xr3:uid="{73F42D88-EBC6-4C98-862C-8700FC2B4625}" name="dfmkey"/>
     <tableColumn id="11" xr3:uid="{6D9259C5-C493-44AF-8751-315AF6A8ACEB}" name="ncmethod"/>
   </tableColumns>
@@ -1068,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C7B812-9642-4C06-A80C-86E8497E4ACA}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1089,7 @@
         <v>77</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>114</v>
@@ -1098,13 +1098,13 @@
         <v>31</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>49</v>
@@ -1113,10 +1113,10 @@
         <v>65</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>102</v>
@@ -1142,7 +1142,7 @@
         <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -1153,13 +1153,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" t="s">
         <v>166</v>
       </c>
-      <c r="B3" t="s">
-        <v>167</v>
-      </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
         <v>122</v>
@@ -1171,18 +1171,18 @@
         <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
         <v>122</v>
@@ -1194,18 +1194,18 @@
         <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" t="s">
         <v>122</v>
@@ -1217,18 +1217,18 @@
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
         <v>122</v>
@@ -1240,18 +1240,18 @@
         <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" t="s">
         <v>122</v>
@@ -1263,18 +1263,18 @@
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
         <v>122</v>
@@ -1286,18 +1286,18 @@
         <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" t="s">
         <v>122</v>
@@ -1309,18 +1309,18 @@
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
         <v>122</v>
@@ -1332,18 +1332,18 @@
         <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D11" t="s">
         <v>122</v>
@@ -1355,18 +1355,18 @@
         <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
         <v>122</v>
@@ -1378,18 +1378,18 @@
         <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
         <v>122</v>
@@ -1401,18 +1401,18 @@
         <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D14" t="s">
         <v>122</v>
@@ -1424,18 +1424,18 @@
         <v>29</v>
       </c>
       <c r="G14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D15" t="s">
         <v>122</v>
@@ -1447,18 +1447,18 @@
         <v>29</v>
       </c>
       <c r="G15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" t="s">
         <v>122</v>
@@ -1470,18 +1470,18 @@
         <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
         <v>122</v>
@@ -1493,18 +1493,18 @@
         <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D18" t="s">
         <v>122</v>
@@ -1516,18 +1516,18 @@
         <v>29</v>
       </c>
       <c r="G18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D19" t="s">
         <v>122</v>
@@ -1539,18 +1539,18 @@
         <v>29</v>
       </c>
       <c r="G19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D20" t="s">
         <v>122</v>
@@ -1567,13 +1567,13 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>199</v>
+      </c>
+      <c r="B21" t="s">
         <v>200</v>
       </c>
-      <c r="B21" t="s">
-        <v>201</v>
-      </c>
       <c r="C21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D21" t="s">
         <v>122</v>
@@ -1590,13 +1590,13 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D22" t="s">
         <v>122</v>
@@ -1608,18 +1608,18 @@
         <v>29</v>
       </c>
       <c r="G22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D23" t="s">
         <v>122</v>
@@ -1631,18 +1631,18 @@
         <v>29</v>
       </c>
       <c r="G23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D24" t="s">
         <v>122</v>
@@ -1654,18 +1654,18 @@
         <v>29</v>
       </c>
       <c r="G24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D25" t="s">
         <v>122</v>
@@ -1677,18 +1677,18 @@
         <v>29</v>
       </c>
       <c r="G25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
         <v>122</v>
@@ -1700,7 +1700,7 @@
         <v>29</v>
       </c>
       <c r="G26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
         <v>110</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
         <v>122</v>
@@ -1723,7 +1723,10 @@
         <v>29</v>
       </c>
       <c r="G27" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1746,9 +1749,12 @@
         <v>29</v>
       </c>
       <c r="G28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1777,6 +1783,9 @@
       <c r="I29" t="s">
         <v>47</v>
       </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
       <c r="M29" t="s">
         <v>64</v>
       </c>
@@ -1956,6 +1965,9 @@
       <c r="G36" t="s">
         <v>30</v>
       </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2216,7 +2228,7 @@
         <v>29</v>
       </c>
       <c r="G47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K47" t="b">
         <v>1</v>
@@ -2239,7 +2251,7 @@
         <v>29</v>
       </c>
       <c r="G48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K48" t="b">
         <v>1</v>
@@ -2262,7 +2274,7 @@
         <v>29</v>
       </c>
       <c r="G49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K49" s="3"/>
     </row>
@@ -2355,7 +2367,7 @@
         <v>29</v>
       </c>
       <c r="G53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K53" t="b">
         <v>1</v>
@@ -2427,7 +2439,7 @@
         <v>29</v>
       </c>
       <c r="G56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K56" t="b">
         <v>1</v>
@@ -2453,7 +2465,7 @@
         <v>29</v>
       </c>
       <c r="G57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more nowcast documentation (v0.10)
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83F3B54-D550-4106-B55A-939C3327E7CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18D4BA0-71B5-4D8F-8E15-FD8EEC345178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="312">
   <si>
     <t>gdp</t>
   </si>
@@ -200,9 +200,6 @@
     <t>spy</t>
   </si>
   <si>
-    <t>SP500</t>
-  </si>
-  <si>
     <t>vix</t>
   </si>
   <si>
@@ -338,9 +335,6 @@
     <t>CSCICP03USM665S</t>
   </si>
   <si>
-    <t>indpro</t>
-  </si>
-  <si>
     <t>Industrial Production index</t>
   </si>
   <si>
@@ -353,15 +347,9 @@
     <t>PCE</t>
   </si>
   <si>
-    <t>dpi</t>
-  </si>
-  <si>
     <t>DSPIC96</t>
   </si>
   <si>
-    <t>Real Disposable Personal Income</t>
-  </si>
-  <si>
     <t>units</t>
   </si>
   <si>
@@ -413,9 +401,6 @@
     <t>pdi</t>
   </si>
   <si>
-    <t>Food and beverages purchased for off-premises consumption</t>
-  </si>
-  <si>
     <t>Exports</t>
   </si>
   <si>
@@ -494,12 +479,6 @@
     <t>SLCEC1</t>
   </si>
   <si>
-    <t>pceq</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures</t>
-  </si>
-  <si>
     <t>pceg</t>
   </si>
   <si>
@@ -509,30 +488,12 @@
     <t>pcegd</t>
   </si>
   <si>
-    <t>pcegf</t>
-  </si>
-  <si>
     <t>pces</t>
   </si>
   <si>
-    <t>Personal Consumption Expenditures: Goods</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Nondurable Goods</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Durable Goods</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Services</t>
-  </si>
-  <si>
     <t>pceshousing</t>
   </si>
   <si>
-    <t>pcestransportation</t>
-  </si>
-  <si>
     <t>pcesfood</t>
   </si>
   <si>
@@ -554,36 +515,9 @@
     <t>pcesnonprofit</t>
   </si>
   <si>
-    <t>Personal Consumption Expenditures: Services: Housing &amp; Utilities</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Services: Health Care</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Services: Transportation</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Services: Recreation</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Services: Food Services &amp; Accomodations</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Services: Financial Services</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Services: Other Services</t>
-  </si>
-  <si>
-    <t>Personal Consumption Expenditures: Services: Nonprofit Services</t>
-  </si>
-  <si>
     <t>Gross Private Domestic Investment</t>
   </si>
   <si>
-    <t>pdinr</t>
-  </si>
-  <si>
     <t>pdir</t>
   </si>
   <si>
@@ -671,9 +605,6 @@
     <t>Consumer Sector</t>
   </si>
   <si>
-    <t>Assets</t>
-  </si>
-  <si>
     <t>Inflation</t>
   </si>
   <si>
@@ -702,6 +633,345 @@
   </si>
   <si>
     <t>EXPGSC1</t>
+  </si>
+  <si>
+    <t>calc</t>
+  </si>
+  <si>
+    <t>DMOTRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DFDHRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DREQRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DODGRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>pcegnfood</t>
+  </si>
+  <si>
+    <t>pcegnclothing</t>
+  </si>
+  <si>
+    <t>pcegngas</t>
+  </si>
+  <si>
+    <t>pcegnother</t>
+  </si>
+  <si>
+    <t>DCLORX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DGOERX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>DONGRX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>mpce</t>
+  </si>
+  <si>
+    <t>mpceg</t>
+  </si>
+  <si>
+    <t>mpcegd</t>
+  </si>
+  <si>
+    <t>mpcegn</t>
+  </si>
+  <si>
+    <t>mpces</t>
+  </si>
+  <si>
+    <t>PCE: Goods: Nondurable Goods</t>
+  </si>
+  <si>
+    <t>PCE: Goods: Durable Goods</t>
+  </si>
+  <si>
+    <t>PCE: Goods</t>
+  </si>
+  <si>
+    <t>PCE: Services</t>
+  </si>
+  <si>
+    <t>PCEDGC96</t>
+  </si>
+  <si>
+    <t>PCENDC96</t>
+  </si>
+  <si>
+    <t>PCESC96</t>
+  </si>
+  <si>
+    <t>DGDSRX1</t>
+  </si>
+  <si>
+    <t>millions of units</t>
+  </si>
+  <si>
+    <t>billions of dollars</t>
+  </si>
+  <si>
+    <t>dollars</t>
+  </si>
+  <si>
+    <t>pdin</t>
+  </si>
+  <si>
+    <t>pcestransport</t>
+  </si>
+  <si>
+    <t>pdinstruct</t>
+  </si>
+  <si>
+    <t>pdinequip</t>
+  </si>
+  <si>
+    <t>pdinip</t>
+  </si>
+  <si>
+    <t>Gross Private Domestic Investment: Nonresidential Investment: Structures</t>
+  </si>
+  <si>
+    <t>Gross Private Domestic Investment: Nonresidential Investment: Equipment</t>
+  </si>
+  <si>
+    <t>Gross Private Domestic Investment: Nonresidential Investment: Intellectual Property</t>
+  </si>
+  <si>
+    <t>B009RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>Y033RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>Y001RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>exg</t>
+  </si>
+  <si>
+    <t>exs</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>ims</t>
+  </si>
+  <si>
+    <t>Exports: Goods</t>
+  </si>
+  <si>
+    <t>Exports: Services</t>
+  </si>
+  <si>
+    <t>Imports: Goods</t>
+  </si>
+  <si>
+    <t>Imports: Services</t>
+  </si>
+  <si>
+    <t>A253RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>A646RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>A255RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>B656RX1Q020SBEA</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>Personal Income</t>
+  </si>
+  <si>
+    <t>po</t>
+  </si>
+  <si>
+    <t>A068RC1</t>
+  </si>
+  <si>
+    <t>RPI</t>
+  </si>
+  <si>
+    <t>Disposable Personal Income</t>
+  </si>
+  <si>
+    <t>Personal Outlays</t>
+  </si>
+  <si>
+    <t>ps</t>
+  </si>
+  <si>
+    <t>pid</t>
+  </si>
+  <si>
+    <t>psr</t>
+  </si>
+  <si>
+    <t>Personal Savings Rate</t>
+  </si>
+  <si>
+    <t>Personal Savings</t>
+  </si>
+  <si>
+    <t>PSAVERT</t>
+  </si>
+  <si>
+    <t>PMSAVE</t>
+  </si>
+  <si>
+    <t>ipi</t>
+  </si>
+  <si>
+    <t>delinqrer</t>
+  </si>
+  <si>
+    <t>Delinquency Rate on Residential Mortgages</t>
+  </si>
+  <si>
+    <t>delinqcc</t>
+  </si>
+  <si>
+    <t>Delinquency Rate on Credit Cards</t>
+  </si>
+  <si>
+    <t>delinqci</t>
+  </si>
+  <si>
+    <t>Delinquency Rate on Commercial &amp; Industrial Loans</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>DRSFRMACBS</t>
+  </si>
+  <si>
+    <t>DRCCLACBS</t>
+  </si>
+  <si>
+    <t>DRBLACBS</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
+    <t>New York Fed: Business Conditions Manufacturing Survey</t>
+  </si>
+  <si>
+    <t>GACDISA066MSFRBNY</t>
+  </si>
+  <si>
+    <t>sny</t>
+  </si>
+  <si>
+    <t>stx</t>
+  </si>
+  <si>
+    <t>BACTSAMFRBDAL</t>
+  </si>
+  <si>
+    <t>pcegdother</t>
+  </si>
+  <si>
+    <t>pcegdrec</t>
+  </si>
+  <si>
+    <t>pcegdfurnish</t>
+  </si>
+  <si>
+    <t>pcegdmotor</t>
+  </si>
+  <si>
+    <t>yahoo</t>
+  </si>
+  <si>
+    <t>cfnai</t>
+  </si>
+  <si>
+    <t>Chicago Fed National Activity Index</t>
+  </si>
+  <si>
+    <t>Labor Market</t>
+  </si>
+  <si>
+    <t>CFNAI</t>
+  </si>
+  <si>
+    <t>Current General Business Activity; Diffusion Index for Texas</t>
+  </si>
+  <si>
+    <t>Personal Consumption</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Durable</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Durable: Motor Vehicles &amp; Parts</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Durable: Furnishings &amp; Durable Household Equipment</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Durable: Recreational Goods &amp; Services</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Durable: Other Durable Goods</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Nondurable Goods</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Nondurable Goods: Food &amp; Beverages for Off-Premises Consumption</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Nondurable Goods: Clothing</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Nondurable Goods: Gasoline &amp; Energy Goods</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Goods: Nondurable Goods: Other Nondurable Goods</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services: Housing &amp; Utilities</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services: Health Care</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services: Transportation</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services: Recreation</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services: Food Services &amp; Accomodations</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services: Financial Services</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services: Other Services</t>
+  </si>
+  <si>
+    <t>Personal Consumptions: Services: Nonprofit Services</t>
   </si>
 </sst>
 </file>
@@ -778,112 +1048,7 @@
   <dxfs count="19">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <color theme="9"/>
       </font>
     </dxf>
     <dxf>
@@ -903,28 +1068,16 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -991,6 +1144,121 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <strike val="0"/>
         <outline val="0"/>
@@ -1050,21 +1318,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B617FE1-E1E8-47F6-ABDE-CBCD504EF9D5}" name="Table1" displayName="Table1" ref="A1:L60" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:L60" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B617FE1-E1E8-47F6-ABDE-CBCD504EF9D5}" name="Table1" displayName="Table1" ref="A1:L88" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:L88" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{60AC762C-6D0B-4264-8E22-97F42B37CA94}" name="varname" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{3D1FA503-3E60-4701-ABF7-5AF7BEE6DD85}" name="fullname" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{C772A0AD-828B-4FC0-84A8-2B91F2102E90}" name="category" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{2C505C57-EF35-4FEB-BC22-0AC6771B8847}" name="source" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{47D8E6E2-3F96-4CD3-A6C7-006EBA2077F7}" name="sckey" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{78E77ED3-181C-477E-B64E-221C0A3DA799}" name="units" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E060E0B9-F2B0-4B1B-96FF-C5F9CEDB6EAC}" name="freq" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{948C1E87-21BA-4E2F-B530-95DCECC8047B}" name="sa" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{1C35A57C-07E1-44AF-A3A8-BA4148FF470E}" name="stat" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{A2B6536A-3838-480C-B021-497CABEA8F6B}" name="display" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{C429D8D4-AEFE-4CFC-B8DA-223FB223EEB7}" name="dfminput" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{542D7F85-BE50-4E7E-8D13-A43E953A4A28}" name="nowcast" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{3D1FA503-3E60-4701-ABF7-5AF7BEE6DD85}" name="fullname" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{C772A0AD-828B-4FC0-84A8-2B91F2102E90}" name="category" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{2C505C57-EF35-4FEB-BC22-0AC6771B8847}" name="source" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{47D8E6E2-3F96-4CD3-A6C7-006EBA2077F7}" name="sckey" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{78E77ED3-181C-477E-B64E-221C0A3DA799}" name="units" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{E060E0B9-F2B0-4B1B-96FF-C5F9CEDB6EAC}" name="freq" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{948C1E87-21BA-4E2F-B530-95DCECC8047B}" name="sa" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{1C35A57C-07E1-44AF-A3A8-BA4148FF470E}" name="stat" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{A2B6536A-3838-480C-B021-497CABEA8F6B}" name="display" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{C429D8D4-AEFE-4CFC-B8DA-223FB223EEB7}" name="dfminput" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{542D7F85-BE50-4E7E-8D13-A43E953A4A28}" name="nowcast" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1367,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C7B812-9642-4C06-A80C-86E8497E4ACA}">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1395,37 +1663,37 @@
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1433,19 +1701,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>32</v>
@@ -1454,30 +1722,30 @@
         <v>29</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>153</v>
+        <v>291</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>32</v>
@@ -1486,30 +1754,30 @@
         <v>29</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>159</v>
+        <v>297</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>32</v>
@@ -1518,30 +1786,30 @@
         <v>29</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>161</v>
+        <v>292</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>32</v>
@@ -1550,30 +1818,30 @@
         <v>29</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>155</v>
+        <v>284</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>160</v>
+        <v>293</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>134</v>
+        <v>200</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>32</v>
@@ -1582,30 +1850,30 @@
         <v>29</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>157</v>
+        <v>283</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>125</v>
+        <v>294</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>32</v>
@@ -1614,30 +1882,30 @@
         <v>29</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>158</v>
+        <v>282</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>162</v>
+        <v>295</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>136</v>
+        <v>202</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>32</v>
@@ -1646,30 +1914,30 @@
         <v>29</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>163</v>
+        <v>281</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>172</v>
+        <v>296</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>137</v>
+        <v>203</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>32</v>
@@ -1678,30 +1946,30 @@
         <v>29</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>173</v>
+        <v>298</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>32</v>
@@ -1710,30 +1978,30 @@
         <v>29</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>164</v>
+        <v>204</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>174</v>
+        <v>299</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>32</v>
@@ -1742,30 +2010,30 @@
         <v>29</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>175</v>
+        <v>300</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>140</v>
+        <v>208</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>32</v>
@@ -1774,30 +2042,30 @@
         <v>29</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>165</v>
+        <v>206</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>176</v>
+        <v>301</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>32</v>
@@ -1806,30 +2074,30 @@
         <v>29</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>167</v>
+        <v>207</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>177</v>
+        <v>302</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>32</v>
@@ -1838,30 +2106,30 @@
         <v>29</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>178</v>
+        <v>303</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>32</v>
@@ -1870,30 +2138,30 @@
         <v>29</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>179</v>
+        <v>304</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>32</v>
@@ -1902,30 +2170,30 @@
         <v>29</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>180</v>
+        <v>305</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>32</v>
@@ -1934,30 +2202,30 @@
         <v>29</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>181</v>
+        <v>228</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>183</v>
+        <v>306</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>32</v>
@@ -1966,30 +2234,30 @@
         <v>29</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>184</v>
+        <v>307</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>32</v>
@@ -1998,94 +2266,94 @@
         <v>29</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>207</v>
-      </c>
       <c r="D20" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>32</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>187</v>
+        <v>309</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>32</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>126</v>
+        <v>310</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>221</v>
+        <v>138</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>32</v>
@@ -2094,30 +2362,30 @@
         <v>29</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>127</v>
+        <v>311</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>220</v>
+        <v>139</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>32</v>
@@ -2126,30 +2394,30 @@
         <v>29</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>32</v>
@@ -2158,30 +2426,30 @@
         <v>29</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>32</v>
@@ -2190,30 +2458,30 @@
         <v>29</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>192</v>
+        <v>229</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>130</v>
+        <v>232</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>32</v>
@@ -2222,138 +2490,129 @@
         <v>29</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>103</v>
+        <v>230</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>104</v>
+        <v>233</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>121</v>
+        <v>236</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>29</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K27" s="5" t="b">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>105</v>
+        <v>231</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>107</v>
+        <v>234</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>106</v>
+        <v>237</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>29</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K28" s="5" t="b">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>75</v>
+        <v>162</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>46</v>
+        <v>141</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>29</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K29" s="5" t="b">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>30</v>
@@ -2361,34 +2620,31 @@
       <c r="J30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="5" t="b">
-        <v>1</v>
-      </c>
       <c r="L30" s="6" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>30</v>
@@ -2397,386 +2653,385 @@
         <v>30</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K32" s="5" t="b">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>19</v>
+        <v>238</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>79</v>
+        <v>242</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>35</v>
+        <v>246</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>20</v>
+        <v>239</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>81</v>
+        <v>243</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>37</v>
+        <v>197</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>22</v>
+        <v>240</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>84</v>
+        <v>244</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>33</v>
+        <v>248</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K36" s="5" t="b">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>23</v>
+        <v>241</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>85</v>
+        <v>245</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>38</v>
+        <v>249</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>25</v>
+        <v>169</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>26</v>
+        <v>170</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>27</v>
+        <v>211</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
+      </c>
+      <c r="K41" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>48</v>
+        <v>212</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>88</v>
+        <v>218</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="7"/>
+        <v>223</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="G42" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="K42" s="5" t="b">
         <v>1</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>49</v>
+        <v>213</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>89</v>
+        <v>217</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>50</v>
+        <v>220</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>44</v>
@@ -2785,66 +3040,68 @@
         <v>29</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="K43" s="5" t="b">
         <v>1</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>51</v>
+        <v>214</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>90</v>
+        <v>216</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F44" s="7"/>
+        <v>221</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="G44" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="K44" s="5" t="b">
         <v>1</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>53</v>
+        <v>215</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>91</v>
+        <v>219</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>54</v>
+        <v>222</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>44</v>
@@ -2853,67 +3110,66 @@
         <v>29</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="K45" s="5" t="b">
         <v>1</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>74</v>
+        <v>251</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>56</v>
+        <v>254</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>114</v>
+        <v>225</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K46" s="5" t="b">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>57</v>
+        <v>258</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>92</v>
+        <v>255</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F47" s="7"/>
+        <v>103</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>225</v>
+      </c>
       <c r="G47" s="6" t="s">
         <v>44</v>
       </c>
@@ -2921,32 +3177,34 @@
         <v>29</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K47" s="5" t="b">
         <v>1</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>59</v>
+        <v>252</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>93</v>
+        <v>256</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F48" s="7"/>
+        <v>253</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>225</v>
+      </c>
       <c r="G48" s="6" t="s">
         <v>44</v>
       </c>
@@ -2954,67 +3212,62 @@
         <v>29</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K48" s="5" t="b">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>61</v>
+        <v>257</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>94</v>
+        <v>261</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F49" s="7"/>
+        <v>263</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>225</v>
+      </c>
       <c r="G49" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H49" s="6" t="b">
-        <v>1</v>
-      </c>
       <c r="I49" s="6" t="s">
         <v>29</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K49" s="6"/>
+        <v>118</v>
+      </c>
       <c r="L49" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>63</v>
+        <v>259</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>95</v>
+        <v>260</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>64</v>
+        <v>262</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>114</v>
+        <v>225</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>44</v>
@@ -3025,37 +3278,34 @@
       <c r="J50" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K50" s="5" t="b">
-        <v>1</v>
-      </c>
       <c r="L50" s="6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J51" s="6" t="s">
         <v>30</v>
@@ -3064,27 +3314,27 @@
         <v>1</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>216</v>
+        <v>105</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>44</v>
@@ -3099,62 +3349,59 @@
         <v>1</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>111</v>
+        <v>43</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K53" s="5" t="b">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>44</v>
@@ -3169,27 +3416,27 @@
         <v>1</v>
       </c>
       <c r="L54" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>217</v>
+        <v>105</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>44</v>
@@ -3200,95 +3447,95 @@
       <c r="J55" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K55" s="5" t="b">
-        <v>1</v>
-      </c>
       <c r="L55" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K56" s="5" t="b">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>122</v>
+        <v>30</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>197</v>
+        <v>22</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>200</v>
+        <v>83</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>205</v>
+        <v>182</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>30</v>
@@ -3296,23 +3543,34 @@
       <c r="J58" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L58" s="6"/>
+      <c r="K58" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>198</v>
+        <v>23</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>201</v>
+        <v>84</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>205</v>
+        <v>182</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="I59" s="6" t="s">
         <v>30</v>
@@ -3320,42 +3578,975 @@
       <c r="J59" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L59" s="6"/>
+      <c r="L59" s="6" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>199</v>
+        <v>24</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>202</v>
+        <v>85</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>205</v>
+        <v>182</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="F60" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K64" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L64" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K65" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L65" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K66" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L66" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K67" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L67" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K68" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K69" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L69" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K70" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L70" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H71" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K72" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K73" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L73" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K74" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K75" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L75" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I60" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L60" s="6"/>
+      <c r="C76" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K76" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K77" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K78" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L78" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L79" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L80" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L81" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I83" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J83" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K83" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L83" s="6"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K84" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L84" s="6"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K85" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L85" s="6"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L86" s="6"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L87" s="6"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L88" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="L2:L60">
-    <cfRule type="expression" dxfId="2" priority="2">
+  <conditionalFormatting sqref="L2:L88">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$K2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K60">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$G3 = "q"</formula>
+  <conditionalFormatting sqref="K2:K88">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$G2 = "q"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added some pretty graphs for nowcasting output (v0.10)
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18D4BA0-71B5-4D8F-8E15-FD8EEC345178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611CCF13-F385-42BF-B3AF-7697F08198CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="params (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="312">
   <si>
     <t>gdp</t>
   </si>
@@ -1045,7 +1046,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="34">
     <dxf>
       <font>
         <color theme="9"/>
@@ -1066,6 +1067,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
@@ -1078,6 +1084,231 @@
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1318,21 +1549,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B617FE1-E1E8-47F6-ABDE-CBCD504EF9D5}" name="Table1" displayName="Table1" ref="A1:L88" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B617FE1-E1E8-47F6-ABDE-CBCD504EF9D5}" name="Table1" displayName="Table1" ref="A1:L87" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:L87" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{60AC762C-6D0B-4264-8E22-97F42B37CA94}" name="varname" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{3D1FA503-3E60-4701-ABF7-5AF7BEE6DD85}" name="fullname" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{C772A0AD-828B-4FC0-84A8-2B91F2102E90}" name="category" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{2C505C57-EF35-4FEB-BC22-0AC6771B8847}" name="source" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{47D8E6E2-3F96-4CD3-A6C7-006EBA2077F7}" name="sckey" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{78E77ED3-181C-477E-B64E-221C0A3DA799}" name="units" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{E060E0B9-F2B0-4B1B-96FF-C5F9CEDB6EAC}" name="freq" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{948C1E87-21BA-4E2F-B530-95DCECC8047B}" name="sa" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{1C35A57C-07E1-44AF-A3A8-BA4148FF470E}" name="stat" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{A2B6536A-3838-480C-B021-497CABEA8F6B}" name="display" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{C429D8D4-AEFE-4CFC-B8DA-223FB223EEB7}" name="dfminput" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{542D7F85-BE50-4E7E-8D13-A43E953A4A28}" name="nowcast" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:L88" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:L88" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{60AC762C-6D0B-4264-8E22-97F42B37CA94}" name="varname" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{3D1FA503-3E60-4701-ABF7-5AF7BEE6DD85}" name="fullname" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{C772A0AD-828B-4FC0-84A8-2B91F2102E90}" name="category" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{2C505C57-EF35-4FEB-BC22-0AC6771B8847}" name="source" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{47D8E6E2-3F96-4CD3-A6C7-006EBA2077F7}" name="sckey" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{78E77ED3-181C-477E-B64E-221C0A3DA799}" name="units" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{E060E0B9-F2B0-4B1B-96FF-C5F9CEDB6EAC}" name="freq" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{948C1E87-21BA-4E2F-B530-95DCECC8047B}" name="sa" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{1C35A57C-07E1-44AF-A3A8-BA4148FF470E}" name="stat" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{A2B6536A-3838-480C-B021-497CABEA8F6B}" name="display" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{C429D8D4-AEFE-4CFC-B8DA-223FB223EEB7}" name="dfminput" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{542D7F85-BE50-4E7E-8D13-A43E953A4A28}" name="nowcast" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="stat" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="display" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1635,10 +1887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C7B812-9642-4C06-A80C-86E8497E4ACA}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4396,6 +4648,2897 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K84" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L84" s="6"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L85" s="6"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L86" s="6"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L87" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="L2:L87">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>$K2=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K87">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$G2 = "q"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"calc"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE13241-3AD3-4AF9-83CF-1259D998F1D6}">
+  <dimension ref="A1:L88"/>
+  <sheetViews>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84:XFD84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K41" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K42" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K43" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K44" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K45" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K47" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K51" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K52" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K54" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J58" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K58" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K64" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L64" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K65" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L65" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K66" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L66" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K67" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L67" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K68" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K69" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L69" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K70" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L70" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H71" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K72" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K73" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L73" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K74" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K75" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L75" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K76" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K77" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K78" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L78" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L79" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L80" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L81" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I83" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J83" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K83" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L83" s="6"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B84" s="5" t="s">
@@ -4533,7 +7676,6 @@
       <c r="L88" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L2:L88">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$K2=TRUE</formula>
@@ -4557,7 +7699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E828C45D-CF7B-424F-B36C-220BE51A990F}">
   <dimension ref="B1:P3"/>
   <sheetViews>
@@ -4638,7 +7780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C702AB-733A-4F06-A26B-F3AA9CF0214F}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>